<commit_message>
second practice measures and some imgs
</commit_message>
<xml_diff>
--- a/lab5/lab5.xlsx
+++ b/lab5/lab5.xlsx
@@ -9,14 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>f, Гц</t>
   </si>
@@ -46,13 +44,31 @@
   <si>
     <t>20lg(k)</t>
   </si>
+  <si>
+    <t>e_c, мВ</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_avg = </t>
+  </si>
+  <si>
+    <t>Теория:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e_max = </t>
+  </si>
+  <si>
+    <t>u_вых = e_c * k_avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,15 +99,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,9 +152,790 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
+          <c:x val="0.15553190017470947"/>
+          <c:y val="4.920175397237022E-2"/>
+          <c:w val="0.81294428439150423"/>
+          <c:h val="0.7655017524007105"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>max</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="plus"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="3000"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                    <a:alpha val="82000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3C65-4FCA-A4EE-FBBDD4FE87B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334418352"/>
+        <c:axId val="334419336"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>exp</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1053</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1190</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1310</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1390</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1490</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1690</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1910</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1980</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C65-4FCA-A4EE-FBBDD4FE87B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>theo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>79.993020163076594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>172.85205056217251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283.61161694181703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>421.78137904167659</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>598.54917184959413</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>732.80319170370865</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>850.27545907605895</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>990.12339642409495</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1157.9409212417381</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1292.1949410958528</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1415.2611259621244</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1560.7029808040818</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1683.7691656703537</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1851.5866904879967</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2008.2163803177971</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2215.1913275928905</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2410.9784398801407</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2567.6081297099408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3C65-4FCA-A4EE-FBBDD4FE87B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334418352"/>
+        <c:axId val="334419336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334418352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>e</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>c</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>, мВ</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47437579197146446"/>
+              <c:y val="0.89719898785106955"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334419336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="334419336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>U</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>вых</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>, мВ</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4285716963951436E-2"/>
+              <c:y val="0.35092460747795745"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334418352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
           <c:x val="0.1293414190741318"/>
           <c:y val="4.920175397237022E-2"/>
-          <c:w val="0.81294428439150423"/>
+          <c:w val="0.81294428439150435"/>
           <c:h val="0.8134059440174769"/>
         </c:manualLayout>
       </c:layout>
@@ -499,6 +1302,15 @@
                   </a:rPr>
                   <a:t> lg(k)</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" sz="1400">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>, дБ</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -660,6 +1472,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1176,7 +2028,560 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1211,19 +2616,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1489,10 +2881,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.43</v>
+      </c>
+      <c r="B2">
+        <v>90.1</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2/A2</f>
+        <v>63.006993006993007</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6">
+        <f>A2*$C$21</f>
+        <v>79.993020163076594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3.09</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C19" si="0">B3/A3</f>
+        <v>64.724919093851142</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F19" si="1">A3*$C$21</f>
+        <v>172.85205056217251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.07</v>
+      </c>
+      <c r="B4">
+        <v>324</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>63.905325443786978</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="1"/>
+        <v>283.61161694181703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7.54</v>
+      </c>
+      <c r="B5">
+        <v>476</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>63.129973474801062</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="1"/>
+        <v>421.78137904167659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10.7</v>
+      </c>
+      <c r="B6">
+        <v>675</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>63.084112149532714</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="1"/>
+        <v>598.54917184959413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>13.1</v>
+      </c>
+      <c r="B7">
+        <v>799</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>60.992366412213741</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
+        <v>732.80319170370865</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15.2</v>
+      </c>
+      <c r="B8">
+        <v>913</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>60.065789473684212</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>850.27545907605895</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>17.7</v>
+      </c>
+      <c r="B9">
+        <v>1053</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>59.491525423728817</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="1"/>
+        <v>990.12339642409495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20.7</v>
+      </c>
+      <c r="B10">
+        <v>1190</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>57.487922705314013</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="1"/>
+        <v>1157.9409212417381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>23.1</v>
+      </c>
+      <c r="B11">
+        <v>1310</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>56.709956709956707</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>1292.1949410958528</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>25.3</v>
+      </c>
+      <c r="B12">
+        <v>1390</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>54.940711462450594</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>1415.2611259621244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>27.9</v>
+      </c>
+      <c r="B13">
+        <v>1490</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>53.405017921146957</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>1560.7029808040818</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>30.1</v>
+      </c>
+      <c r="B14">
+        <v>1580</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>52.491694352159463</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="1"/>
+        <v>1683.7691656703537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>33.1</v>
+      </c>
+      <c r="B15">
+        <v>1690</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>51.057401812688816</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>1851.5866904879967</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>35.9</v>
+      </c>
+      <c r="B16">
+        <v>1750</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>48.746518105849582</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="1"/>
+        <v>2008.2163803177971</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>39.6</v>
+      </c>
+      <c r="B17">
+        <v>1830</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>46.212121212121211</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="1"/>
+        <v>2215.1913275928905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>43.1</v>
+      </c>
+      <c r="B18">
+        <v>1910</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>44.315545243619489</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="1"/>
+        <v>2410.9784398801407</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>45.9</v>
+      </c>
+      <c r="B19">
+        <v>1980</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>43.137254901960787</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="1"/>
+        <v>2567.6081297099408</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5">
+        <f>AVERAGE(C2:C19)</f>
+        <v>55.939174939214404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>30.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>